<commit_message>
Realized the classification ID's into the spreadsheet
</commit_message>
<xml_diff>
--- a/CHTN East Vocabulary Modifier - Classifications.xlsx
+++ b/CHTN East Vocabulary Modifier - Classifications.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="13440"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="voc_site_classifications" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">voc_site_classifications!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">voc_site_classifications!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="249">
   <si>
     <t>ARM</t>
   </si>
@@ -708,13 +713,70 @@
   </si>
   <si>
     <t>Anatomic Site</t>
+  </si>
+  <si>
+    <t>Classification Id</t>
+  </si>
+  <si>
+    <t>CL1</t>
+  </si>
+  <si>
+    <t>CL2</t>
+  </si>
+  <si>
+    <t>CL3</t>
+  </si>
+  <si>
+    <t>CL4</t>
+  </si>
+  <si>
+    <t>CL5</t>
+  </si>
+  <si>
+    <t>CL6</t>
+  </si>
+  <si>
+    <t>CL7</t>
+  </si>
+  <si>
+    <t>CL8</t>
+  </si>
+  <si>
+    <t>CL9</t>
+  </si>
+  <si>
+    <t>CL10</t>
+  </si>
+  <si>
+    <t>CL11</t>
+  </si>
+  <si>
+    <t>CL12</t>
+  </si>
+  <si>
+    <t>CL13</t>
+  </si>
+  <si>
+    <t>CL14</t>
+  </si>
+  <si>
+    <t>CL15</t>
+  </si>
+  <si>
+    <t>CL16</t>
+  </si>
+  <si>
+    <t>CL17</t>
+  </si>
+  <si>
+    <t>CL18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -846,6 +908,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1148,7 +1226,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1191,18 +1269,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1231,11 +1304,13 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1543,47 +1618,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>228</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>229</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:5">
+      <c r="A2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>88</v>
       </c>
       <c r="D2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:5">
+      <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -1593,11 +1675,14 @@
         <v>129</v>
       </c>
       <c r="D3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:5">
+      <c r="A4">
         <v>5</v>
       </c>
       <c r="B4" t="s">
@@ -1607,11 +1692,14 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:5">
+      <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" t="s">
@@ -1621,11 +1709,14 @@
         <v>33</v>
       </c>
       <c r="D5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:5">
+      <c r="A6">
         <v>7</v>
       </c>
       <c r="B6" t="s">
@@ -1635,11 +1726,14 @@
         <v>37</v>
       </c>
       <c r="D6" t="s">
+        <v>234</v>
+      </c>
+      <c r="E6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:5">
+      <c r="A7">
         <v>8</v>
       </c>
       <c r="B7" t="s">
@@ -1649,11 +1743,14 @@
         <v>90</v>
       </c>
       <c r="D7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:5">
+      <c r="A8">
         <v>9</v>
       </c>
       <c r="B8" t="s">
@@ -1663,11 +1760,14 @@
         <v>39</v>
       </c>
       <c r="D8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:5">
+      <c r="A9">
         <v>10</v>
       </c>
       <c r="B9" t="s">
@@ -1677,11 +1777,14 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:5">
+      <c r="A10">
         <v>11</v>
       </c>
       <c r="B10" t="s">
@@ -1691,11 +1794,14 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:5">
+      <c r="A11">
         <v>12</v>
       </c>
       <c r="B11" t="s">
@@ -1705,11 +1811,14 @@
         <v>42</v>
       </c>
       <c r="D11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:5">
+      <c r="A12">
         <v>13</v>
       </c>
       <c r="B12" t="s">
@@ -1719,11 +1828,14 @@
         <v>85</v>
       </c>
       <c r="D12" t="s">
+        <v>238</v>
+      </c>
+      <c r="E12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:5">
+      <c r="A13">
         <v>14</v>
       </c>
       <c r="B13" t="s">
@@ -1733,11 +1845,14 @@
         <v>120</v>
       </c>
       <c r="D13" t="s">
+        <v>239</v>
+      </c>
+      <c r="E13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14" spans="1:5">
+      <c r="A14">
         <v>15</v>
       </c>
       <c r="B14" t="s">
@@ -1747,11 +1862,14 @@
         <v>86</v>
       </c>
       <c r="D14" t="s">
+        <v>238</v>
+      </c>
+      <c r="E14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="15" spans="1:5">
+      <c r="A15">
         <v>16</v>
       </c>
       <c r="B15" t="s">
@@ -1761,11 +1879,14 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
+        <v>240</v>
+      </c>
+      <c r="E15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16" spans="1:5">
+      <c r="A16">
         <v>17</v>
       </c>
       <c r="B16" t="s">
@@ -1775,11 +1896,14 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
+        <v>240</v>
+      </c>
+      <c r="E16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17" spans="1:5">
+      <c r="A17">
         <v>18</v>
       </c>
       <c r="B17" t="s">
@@ -1789,11 +1913,14 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="18" spans="1:5">
+      <c r="A18">
         <v>19</v>
       </c>
       <c r="B18" t="s">
@@ -1803,11 +1930,14 @@
         <v>112</v>
       </c>
       <c r="D18" t="s">
+        <v>242</v>
+      </c>
+      <c r="E18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19" spans="1:5">
+      <c r="A19">
         <v>20</v>
       </c>
       <c r="B19" t="s">
@@ -1817,11 +1947,14 @@
         <v>22</v>
       </c>
       <c r="D19" t="s">
+        <v>233</v>
+      </c>
+      <c r="E19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20" spans="1:5">
+      <c r="A20">
         <v>21</v>
       </c>
       <c r="B20" t="s">
@@ -1831,11 +1964,14 @@
         <v>121</v>
       </c>
       <c r="D20" t="s">
+        <v>239</v>
+      </c>
+      <c r="E20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21" spans="1:5">
+      <c r="A21">
         <v>22</v>
       </c>
       <c r="B21" t="s">
@@ -1845,11 +1981,14 @@
         <v>55</v>
       </c>
       <c r="D21" t="s">
+        <v>243</v>
+      </c>
+      <c r="E21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="22" spans="1:5">
+      <c r="A22">
         <v>23</v>
       </c>
       <c r="B22" t="s">
@@ -1859,11 +1998,14 @@
         <v>117</v>
       </c>
       <c r="D22" t="s">
+        <v>239</v>
+      </c>
+      <c r="E22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="23" spans="1:5">
+      <c r="A23">
         <v>24</v>
       </c>
       <c r="B23" t="s">
@@ -1873,11 +2015,14 @@
         <v>34</v>
       </c>
       <c r="D23" t="s">
+        <v>234</v>
+      </c>
+      <c r="E23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="24" spans="1:5">
+      <c r="A24">
         <v>25</v>
       </c>
       <c r="B24" t="s">
@@ -1887,11 +2032,14 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
+        <v>234</v>
+      </c>
+      <c r="E24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="25" spans="1:5">
+      <c r="A25">
         <v>26</v>
       </c>
       <c r="B25" t="s">
@@ -1901,11 +2049,14 @@
         <v>131</v>
       </c>
       <c r="D25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E25" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="26" spans="1:5">
+      <c r="A26">
         <v>27</v>
       </c>
       <c r="B26" t="s">
@@ -1915,11 +2066,14 @@
         <v>94</v>
       </c>
       <c r="D26" t="s">
+        <v>231</v>
+      </c>
+      <c r="E26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="27" spans="1:5">
+      <c r="A27">
         <v>28</v>
       </c>
       <c r="B27" t="s">
@@ -1929,11 +2083,14 @@
         <v>58</v>
       </c>
       <c r="D27" t="s">
+        <v>243</v>
+      </c>
+      <c r="E27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="28" spans="1:5">
+      <c r="A28">
         <v>29</v>
       </c>
       <c r="B28" t="s">
@@ -1943,11 +2100,14 @@
         <v>51</v>
       </c>
       <c r="D28" t="s">
+        <v>237</v>
+      </c>
+      <c r="E28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="29" spans="1:5">
+      <c r="A29">
         <v>30</v>
       </c>
       <c r="B29" t="s">
@@ -1957,11 +2117,14 @@
         <v>32</v>
       </c>
       <c r="D29" t="s">
+        <v>234</v>
+      </c>
+      <c r="E29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="30" spans="1:5">
+      <c r="A30">
         <v>31</v>
       </c>
       <c r="B30" t="s">
@@ -1971,11 +2134,14 @@
         <v>73</v>
       </c>
       <c r="D30" t="s">
+        <v>244</v>
+      </c>
+      <c r="E30" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31" spans="1:5">
+      <c r="A31">
         <v>32</v>
       </c>
       <c r="B31" t="s">
@@ -1985,11 +2151,14 @@
         <v>60</v>
       </c>
       <c r="D31" t="s">
+        <v>243</v>
+      </c>
+      <c r="E31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="32" spans="1:5">
+      <c r="A32">
         <v>33</v>
       </c>
       <c r="B32" t="s">
@@ -1999,11 +2168,14 @@
         <v>56</v>
       </c>
       <c r="D32" t="s">
+        <v>243</v>
+      </c>
+      <c r="E32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="33" spans="1:5">
+      <c r="A33">
         <v>34</v>
       </c>
       <c r="B33" t="s">
@@ -2013,11 +2185,14 @@
         <v>93</v>
       </c>
       <c r="D33" t="s">
+        <v>231</v>
+      </c>
+      <c r="E33" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+    <row r="34" spans="1:5">
+      <c r="A34">
         <v>35</v>
       </c>
       <c r="B34" t="s">
@@ -2027,11 +2202,14 @@
         <v>119</v>
       </c>
       <c r="D34" t="s">
+        <v>239</v>
+      </c>
+      <c r="E34" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="35" spans="1:5">
+      <c r="A35">
         <v>36</v>
       </c>
       <c r="B35" t="s">
@@ -2041,11 +2219,14 @@
         <v>47</v>
       </c>
       <c r="D35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="36" spans="1:5">
+      <c r="A36">
         <v>37</v>
       </c>
       <c r="B36" t="s">
@@ -2055,11 +2236,14 @@
         <v>29</v>
       </c>
       <c r="D36" t="s">
+        <v>234</v>
+      </c>
+      <c r="E36" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="37" spans="1:5">
+      <c r="A37">
         <v>38</v>
       </c>
       <c r="B37" t="s">
@@ -2069,11 +2253,14 @@
         <v>96</v>
       </c>
       <c r="D37" t="s">
+        <v>245</v>
+      </c>
+      <c r="E37" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+    <row r="38" spans="1:5">
+      <c r="A38">
         <v>39</v>
       </c>
       <c r="B38" t="s">
@@ -2083,11 +2270,14 @@
         <v>27</v>
       </c>
       <c r="D38" t="s">
+        <v>234</v>
+      </c>
+      <c r="E38" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="39" spans="1:5">
+      <c r="A39">
         <v>40</v>
       </c>
       <c r="B39" t="s">
@@ -2097,11 +2287,14 @@
         <v>7</v>
       </c>
       <c r="D39" t="s">
+        <v>236</v>
+      </c>
+      <c r="E39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="40" spans="1:5">
+      <c r="A40">
         <v>41</v>
       </c>
       <c r="B40" t="s">
@@ -2111,11 +2304,14 @@
         <v>6</v>
       </c>
       <c r="D40" t="s">
+        <v>236</v>
+      </c>
+      <c r="E40" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+    <row r="41" spans="1:5">
+      <c r="A41">
         <v>42</v>
       </c>
       <c r="B41" t="s">
@@ -2125,11 +2321,14 @@
         <v>81</v>
       </c>
       <c r="D41" t="s">
+        <v>238</v>
+      </c>
+      <c r="E41" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="42" spans="1:5">
+      <c r="A42">
         <v>43</v>
       </c>
       <c r="B42" t="s">
@@ -2139,11 +2338,14 @@
         <v>80</v>
       </c>
       <c r="D42" t="s">
+        <v>238</v>
+      </c>
+      <c r="E42" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+    <row r="43" spans="1:5">
+      <c r="A43">
         <v>44</v>
       </c>
       <c r="B43" t="s">
@@ -2153,11 +2355,14 @@
         <v>101</v>
       </c>
       <c r="D43" t="s">
+        <v>246</v>
+      </c>
+      <c r="E43" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+    <row r="44" spans="1:5">
+      <c r="A44">
         <v>45</v>
       </c>
       <c r="B44" t="s">
@@ -2167,11 +2372,14 @@
         <v>102</v>
       </c>
       <c r="D44" t="s">
+        <v>246</v>
+      </c>
+      <c r="E44" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+    <row r="45" spans="1:5">
+      <c r="A45">
         <v>46</v>
       </c>
       <c r="B45" t="s">
@@ -2181,11 +2389,14 @@
         <v>100</v>
       </c>
       <c r="D45" t="s">
+        <v>246</v>
+      </c>
+      <c r="E45" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+    <row r="46" spans="1:5">
+      <c r="A46">
         <v>47</v>
       </c>
       <c r="B46" t="s">
@@ -2195,11 +2406,14 @@
         <v>98</v>
       </c>
       <c r="D46" t="s">
+        <v>246</v>
+      </c>
+      <c r="E46" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+    <row r="47" spans="1:5">
+      <c r="A47">
         <v>48</v>
       </c>
       <c r="B47" t="s">
@@ -2209,11 +2423,14 @@
         <v>43</v>
       </c>
       <c r="D47" t="s">
+        <v>237</v>
+      </c>
+      <c r="E47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+    <row r="48" spans="1:5">
+      <c r="A48">
         <v>49</v>
       </c>
       <c r="B48" t="s">
@@ -2223,11 +2440,14 @@
         <v>74</v>
       </c>
       <c r="D48" t="s">
+        <v>244</v>
+      </c>
+      <c r="E48" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+    <row r="49" spans="1:5">
+      <c r="A49">
         <v>50</v>
       </c>
       <c r="B49" t="s">
@@ -2237,11 +2457,14 @@
         <v>118</v>
       </c>
       <c r="D49" t="s">
+        <v>239</v>
+      </c>
+      <c r="E49" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+    <row r="50" spans="1:5">
+      <c r="A50">
         <v>51</v>
       </c>
       <c r="B50" t="s">
@@ -2251,11 +2474,14 @@
         <v>79</v>
       </c>
       <c r="D50" t="s">
+        <v>238</v>
+      </c>
+      <c r="E50" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+    <row r="51" spans="1:5">
+      <c r="A51">
         <v>52</v>
       </c>
       <c r="B51" t="s">
@@ -2265,11 +2491,14 @@
         <v>135</v>
       </c>
       <c r="D51" t="s">
+        <v>232</v>
+      </c>
+      <c r="E51" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+    <row r="52" spans="1:5">
+      <c r="A52">
         <v>53</v>
       </c>
       <c r="B52" t="s">
@@ -2279,11 +2508,14 @@
         <v>105</v>
       </c>
       <c r="D52" t="s">
+        <v>247</v>
+      </c>
+      <c r="E52" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+    <row r="53" spans="1:5">
+      <c r="A53">
         <v>54</v>
       </c>
       <c r="B53" t="s">
@@ -2293,11 +2525,14 @@
         <v>30</v>
       </c>
       <c r="D53" t="s">
+        <v>234</v>
+      </c>
+      <c r="E53" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+    <row r="54" spans="1:5">
+      <c r="A54">
         <v>55</v>
       </c>
       <c r="B54" t="s">
@@ -2307,11 +2542,14 @@
         <v>114</v>
       </c>
       <c r="D54" t="s">
+        <v>242</v>
+      </c>
+      <c r="E54" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+    <row r="55" spans="1:5">
+      <c r="A55">
         <v>56</v>
       </c>
       <c r="B55" t="s">
@@ -2321,11 +2559,14 @@
         <v>91</v>
       </c>
       <c r="D55" t="s">
+        <v>231</v>
+      </c>
+      <c r="E55" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+    <row r="56" spans="1:5">
+      <c r="A56">
         <v>57</v>
       </c>
       <c r="B56" t="s">
@@ -2335,11 +2576,14 @@
         <v>82</v>
       </c>
       <c r="D56" t="s">
+        <v>238</v>
+      </c>
+      <c r="E56" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+    <row r="57" spans="1:5">
+      <c r="A57">
         <v>58</v>
       </c>
       <c r="B57" t="s">
@@ -2349,11 +2593,14 @@
         <v>83</v>
       </c>
       <c r="D57" t="s">
+        <v>238</v>
+      </c>
+      <c r="E57" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+    <row r="58" spans="1:5">
+      <c r="A58">
         <v>59</v>
       </c>
       <c r="B58" t="s">
@@ -2363,11 +2610,14 @@
         <v>87</v>
       </c>
       <c r="D58" t="s">
+        <v>238</v>
+      </c>
+      <c r="E58" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+    <row r="59" spans="1:5">
+      <c r="A59">
         <v>60</v>
       </c>
       <c r="B59" t="s">
@@ -2377,11 +2627,14 @@
         <v>113</v>
       </c>
       <c r="D59" t="s">
+        <v>242</v>
+      </c>
+      <c r="E59" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+    <row r="60" spans="1:5">
+      <c r="A60">
         <v>61</v>
       </c>
       <c r="B60" t="s">
@@ -2391,11 +2644,14 @@
         <v>122</v>
       </c>
       <c r="D60" t="s">
+        <v>248</v>
+      </c>
+      <c r="E60" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+    <row r="61" spans="1:5">
+      <c r="A61">
         <v>62</v>
       </c>
       <c r="B61" t="s">
@@ -2405,11 +2661,14 @@
         <v>126</v>
       </c>
       <c r="D61" t="s">
+        <v>232</v>
+      </c>
+      <c r="E61" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+    <row r="62" spans="1:5">
+      <c r="A62">
         <v>63</v>
       </c>
       <c r="B62" t="s">
@@ -2419,11 +2678,14 @@
         <v>127</v>
       </c>
       <c r="D62" t="s">
+        <v>232</v>
+      </c>
+      <c r="E62" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+    <row r="63" spans="1:5">
+      <c r="A63">
         <v>64</v>
       </c>
       <c r="B63" t="s">
@@ -2433,11 +2695,14 @@
         <v>84</v>
       </c>
       <c r="D63" t="s">
+        <v>238</v>
+      </c>
+      <c r="E63" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+    <row r="64" spans="1:5">
+      <c r="A64">
         <v>65</v>
       </c>
       <c r="B64" t="s">
@@ -2447,11 +2712,14 @@
         <v>128</v>
       </c>
       <c r="D64" t="s">
+        <v>232</v>
+      </c>
+      <c r="E64" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+    <row r="65" spans="1:5">
+      <c r="A65">
         <v>66</v>
       </c>
       <c r="B65" t="s">
@@ -2461,11 +2729,14 @@
         <v>139</v>
       </c>
       <c r="D65" t="s">
+        <v>232</v>
+      </c>
+      <c r="E65" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+    <row r="66" spans="1:5">
+      <c r="A66">
         <v>67</v>
       </c>
       <c r="B66" t="s">
@@ -2475,11 +2746,14 @@
         <v>71</v>
       </c>
       <c r="D66" t="s">
+        <v>244</v>
+      </c>
+      <c r="E66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+    <row r="67" spans="1:5">
+      <c r="A67">
         <v>68</v>
       </c>
       <c r="B67" t="s">
@@ -2489,11 +2763,14 @@
         <v>15</v>
       </c>
       <c r="D67" t="s">
+        <v>240</v>
+      </c>
+      <c r="E67" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+    <row r="68" spans="1:5">
+      <c r="A68">
         <v>69</v>
       </c>
       <c r="B68" t="s">
@@ -2503,11 +2780,14 @@
         <v>14</v>
       </c>
       <c r="D68" t="s">
+        <v>240</v>
+      </c>
+      <c r="E68" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+    <row r="69" spans="1:5">
+      <c r="A69">
         <v>70</v>
       </c>
       <c r="B69" t="s">
@@ -2517,11 +2797,14 @@
         <v>16</v>
       </c>
       <c r="D69" t="s">
+        <v>240</v>
+      </c>
+      <c r="E69" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+    <row r="70" spans="1:5">
+      <c r="A70">
         <v>71</v>
       </c>
       <c r="B70" t="s">
@@ -2531,11 +2814,14 @@
         <v>23</v>
       </c>
       <c r="D70" t="s">
+        <v>233</v>
+      </c>
+      <c r="E70" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+    <row r="71" spans="1:5">
+      <c r="A71">
         <v>72</v>
       </c>
       <c r="B71" t="s">
@@ -2545,11 +2831,14 @@
         <v>9</v>
       </c>
       <c r="D71" t="s">
+        <v>240</v>
+      </c>
+      <c r="E71" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+    <row r="72" spans="1:5">
+      <c r="A72">
         <v>73</v>
       </c>
       <c r="B72" t="s">
@@ -2559,11 +2848,14 @@
         <v>140</v>
       </c>
       <c r="D72" t="s">
+        <v>232</v>
+      </c>
+      <c r="E72" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+    <row r="73" spans="1:5">
+      <c r="A73">
         <v>74</v>
       </c>
       <c r="B73" t="s">
@@ -2573,11 +2865,14 @@
         <v>66</v>
       </c>
       <c r="D73" t="s">
+        <v>244</v>
+      </c>
+      <c r="E73" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+    <row r="74" spans="1:5">
+      <c r="A74">
         <v>75</v>
       </c>
       <c r="B74" t="s">
@@ -2587,11 +2882,14 @@
         <v>67</v>
       </c>
       <c r="D74" t="s">
+        <v>244</v>
+      </c>
+      <c r="E74" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+    <row r="75" spans="1:5">
+      <c r="A75">
         <v>76</v>
       </c>
       <c r="B75" t="s">
@@ -2601,11 +2899,14 @@
         <v>52</v>
       </c>
       <c r="D75" t="s">
+        <v>243</v>
+      </c>
+      <c r="E75" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+    <row r="76" spans="1:5">
+      <c r="A76">
         <v>77</v>
       </c>
       <c r="B76" t="s">
@@ -2615,11 +2916,14 @@
         <v>38</v>
       </c>
       <c r="D76" t="s">
+        <v>234</v>
+      </c>
+      <c r="E76" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+    <row r="77" spans="1:5">
+      <c r="A77">
         <v>78</v>
       </c>
       <c r="B77" t="s">
@@ -2629,11 +2933,14 @@
         <v>20</v>
       </c>
       <c r="D77" t="s">
+        <v>233</v>
+      </c>
+      <c r="E77" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+    <row r="78" spans="1:5">
+      <c r="A78">
         <v>79</v>
       </c>
       <c r="B78" t="s">
@@ -2643,11 +2950,14 @@
         <v>50</v>
       </c>
       <c r="D78" t="s">
+        <v>237</v>
+      </c>
+      <c r="E78" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+    <row r="79" spans="1:5">
+      <c r="A79">
         <v>80</v>
       </c>
       <c r="B79" t="s">
@@ -2657,11 +2967,14 @@
         <v>138</v>
       </c>
       <c r="D79" t="s">
+        <v>232</v>
+      </c>
+      <c r="E79" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+    <row r="80" spans="1:5">
+      <c r="A80">
         <v>81</v>
       </c>
       <c r="B80" t="s">
@@ -2671,11 +2984,14 @@
         <v>137</v>
       </c>
       <c r="D80" t="s">
+        <v>232</v>
+      </c>
+      <c r="E80" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+    <row r="81" spans="1:5">
+      <c r="A81">
         <v>82</v>
       </c>
       <c r="B81" t="s">
@@ -2685,11 +3001,14 @@
         <v>136</v>
       </c>
       <c r="D81" t="s">
+        <v>232</v>
+      </c>
+      <c r="E81" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+    <row r="82" spans="1:5">
+      <c r="A82">
         <v>83</v>
       </c>
       <c r="B82" t="s">
@@ -2699,11 +3018,14 @@
         <v>17</v>
       </c>
       <c r="D82" t="s">
+        <v>233</v>
+      </c>
+      <c r="E82" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+    <row r="83" spans="1:5">
+      <c r="A83">
         <v>84</v>
       </c>
       <c r="B83" t="s">
@@ -2713,11 +3035,14 @@
         <v>54</v>
       </c>
       <c r="D83" t="s">
+        <v>243</v>
+      </c>
+      <c r="E83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+    <row r="84" spans="1:5">
+      <c r="A84">
         <v>85</v>
       </c>
       <c r="B84" t="s">
@@ -2727,11 +3052,14 @@
         <v>77</v>
       </c>
       <c r="D84" t="s">
+        <v>238</v>
+      </c>
+      <c r="E84" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+    <row r="85" spans="1:5">
+      <c r="A85">
         <v>86</v>
       </c>
       <c r="B85" t="s">
@@ -2741,11 +3069,14 @@
         <v>134</v>
       </c>
       <c r="D85" t="s">
+        <v>232</v>
+      </c>
+      <c r="E85" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+    <row r="86" spans="1:5">
+      <c r="A86">
         <v>87</v>
       </c>
       <c r="B86" t="s">
@@ -2755,11 +3086,14 @@
         <v>44</v>
       </c>
       <c r="D86" t="s">
+        <v>237</v>
+      </c>
+      <c r="E86" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+    <row r="87" spans="1:5">
+      <c r="A87">
         <v>88</v>
       </c>
       <c r="B87" t="s">
@@ -2769,11 +3103,14 @@
         <v>24</v>
       </c>
       <c r="D87" t="s">
+        <v>234</v>
+      </c>
+      <c r="E87" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+    <row r="88" spans="1:5">
+      <c r="A88">
         <v>89</v>
       </c>
       <c r="B88" t="s">
@@ -2783,11 +3120,14 @@
         <v>64</v>
       </c>
       <c r="D88" t="s">
+        <v>244</v>
+      </c>
+      <c r="E88" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+    <row r="89" spans="1:5">
+      <c r="A89">
         <v>90</v>
       </c>
       <c r="B89" t="s">
@@ -2797,11 +3137,14 @@
         <v>92</v>
       </c>
       <c r="D89" t="s">
+        <v>231</v>
+      </c>
+      <c r="E89" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+    <row r="90" spans="1:5">
+      <c r="A90">
         <v>91</v>
       </c>
       <c r="B90" t="s">
@@ -2811,11 +3154,14 @@
         <v>124</v>
       </c>
       <c r="D90" t="s">
+        <v>232</v>
+      </c>
+      <c r="E90" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+    <row r="91" spans="1:5">
+      <c r="A91">
         <v>92</v>
       </c>
       <c r="B91" t="s">
@@ -2825,11 +3171,14 @@
         <v>40</v>
       </c>
       <c r="D91" t="s">
+        <v>237</v>
+      </c>
+      <c r="E91" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+    <row r="92" spans="1:5">
+      <c r="A92">
         <v>93</v>
       </c>
       <c r="B92" t="s">
@@ -2839,11 +3188,14 @@
         <v>70</v>
       </c>
       <c r="D92" t="s">
+        <v>244</v>
+      </c>
+      <c r="E92" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+    <row r="93" spans="1:5">
+      <c r="A93">
         <v>94</v>
       </c>
       <c r="B93" t="s">
@@ -2853,11 +3205,14 @@
         <v>130</v>
       </c>
       <c r="D93" t="s">
+        <v>232</v>
+      </c>
+      <c r="E93" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+    <row r="94" spans="1:5">
+      <c r="A94">
         <v>95</v>
       </c>
       <c r="B94" t="s">
@@ -2867,11 +3222,14 @@
         <v>123</v>
       </c>
       <c r="D94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E94" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+    <row r="95" spans="1:5">
+      <c r="A95">
         <v>96</v>
       </c>
       <c r="B95" t="s">
@@ -2881,11 +3239,14 @@
         <v>31</v>
       </c>
       <c r="D95" t="s">
+        <v>234</v>
+      </c>
+      <c r="E95" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+    <row r="96" spans="1:5">
+      <c r="A96">
         <v>97</v>
       </c>
       <c r="B96" t="s">
@@ -2895,11 +3256,14 @@
         <v>26</v>
       </c>
       <c r="D96" t="s">
+        <v>234</v>
+      </c>
+      <c r="E96" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+    <row r="97" spans="1:5">
+      <c r="A97">
         <v>98</v>
       </c>
       <c r="B97" t="s">
@@ -2909,11 +3273,14 @@
         <v>125</v>
       </c>
       <c r="D97" t="s">
+        <v>232</v>
+      </c>
+      <c r="E97" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+    <row r="98" spans="1:5">
+      <c r="A98">
         <v>99</v>
       </c>
       <c r="B98" t="s">
@@ -2923,11 +3290,14 @@
         <v>11</v>
       </c>
       <c r="D98" t="s">
+        <v>240</v>
+      </c>
+      <c r="E98" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+    <row r="99" spans="1:5">
+      <c r="A99">
         <v>100</v>
       </c>
       <c r="B99" t="s">
@@ -2937,11 +3307,14 @@
         <v>75</v>
       </c>
       <c r="D99" t="s">
+        <v>238</v>
+      </c>
+      <c r="E99" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+    <row r="100" spans="1:5">
+      <c r="A100">
         <v>101</v>
       </c>
       <c r="B100" t="s">
@@ -2951,11 +3324,14 @@
         <v>28</v>
       </c>
       <c r="D100" t="s">
+        <v>234</v>
+      </c>
+      <c r="E100" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+    <row r="101" spans="1:5">
+      <c r="A101">
         <v>102</v>
       </c>
       <c r="B101" t="s">
@@ -2965,11 +3341,14 @@
         <v>36</v>
       </c>
       <c r="D101" t="s">
+        <v>234</v>
+      </c>
+      <c r="E101" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+    <row r="102" spans="1:5">
+      <c r="A102">
         <v>103</v>
       </c>
       <c r="B102" t="s">
@@ -2979,11 +3358,14 @@
         <v>106</v>
       </c>
       <c r="D102" t="s">
+        <v>247</v>
+      </c>
+      <c r="E102" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+    <row r="103" spans="1:5">
+      <c r="A103">
         <v>104</v>
       </c>
       <c r="B103" t="s">
@@ -2993,11 +3375,14 @@
         <v>107</v>
       </c>
       <c r="D103" t="s">
+        <v>247</v>
+      </c>
+      <c r="E103" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+    <row r="104" spans="1:5">
+      <c r="A104">
         <v>105</v>
       </c>
       <c r="B104" t="s">
@@ -3007,11 +3392,14 @@
         <v>132</v>
       </c>
       <c r="D104" t="s">
+        <v>232</v>
+      </c>
+      <c r="E104" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+    <row r="105" spans="1:5">
+      <c r="A105">
         <v>106</v>
       </c>
       <c r="B105" t="s">
@@ -3021,11 +3409,14 @@
         <v>133</v>
       </c>
       <c r="D105" t="s">
+        <v>232</v>
+      </c>
+      <c r="E105" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+    <row r="106" spans="1:5">
+      <c r="A106">
         <v>107</v>
       </c>
       <c r="B106" t="s">
@@ -3035,11 +3426,14 @@
         <v>48</v>
       </c>
       <c r="D106" t="s">
+        <v>237</v>
+      </c>
+      <c r="E106" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+    <row r="107" spans="1:5">
+      <c r="A107">
         <v>108</v>
       </c>
       <c r="B107" t="s">
@@ -3049,11 +3443,14 @@
         <v>78</v>
       </c>
       <c r="D107" t="s">
+        <v>238</v>
+      </c>
+      <c r="E107" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+    <row r="108" spans="1:5">
+      <c r="A108">
         <v>109</v>
       </c>
       <c r="B108" t="s">
@@ -3063,11 +3460,14 @@
         <v>21</v>
       </c>
       <c r="D108" t="s">
+        <v>233</v>
+      </c>
+      <c r="E108" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+    <row r="109" spans="1:5">
+      <c r="A109">
         <v>110</v>
       </c>
       <c r="B109" t="s">
@@ -3077,11 +3477,14 @@
         <v>108</v>
       </c>
       <c r="D109" t="s">
+        <v>247</v>
+      </c>
+      <c r="E109" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+    <row r="110" spans="1:5">
+      <c r="A110">
         <v>111</v>
       </c>
       <c r="B110" t="s">
@@ -3091,11 +3494,14 @@
         <v>68</v>
       </c>
       <c r="D110" t="s">
+        <v>244</v>
+      </c>
+      <c r="E110" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+    <row r="111" spans="1:5">
+      <c r="A111">
         <v>113</v>
       </c>
       <c r="B111" t="s">
@@ -3105,11 +3511,14 @@
         <v>72</v>
       </c>
       <c r="D111" t="s">
+        <v>244</v>
+      </c>
+      <c r="E111" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+    <row r="112" spans="1:5">
+      <c r="A112">
         <v>112</v>
       </c>
       <c r="B112" t="s">
@@ -3119,11 +3528,14 @@
         <v>69</v>
       </c>
       <c r="D112" t="s">
+        <v>244</v>
+      </c>
+      <c r="E112" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
+    <row r="113" spans="1:5">
+      <c r="A113">
         <v>114</v>
       </c>
       <c r="B113" t="s">
@@ -3133,11 +3545,14 @@
         <v>111</v>
       </c>
       <c r="D113" t="s">
+        <v>242</v>
+      </c>
+      <c r="E113" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+    <row r="114" spans="1:5">
+      <c r="A114">
         <v>115</v>
       </c>
       <c r="B114" t="s">
@@ -3147,11 +3562,14 @@
         <v>109</v>
       </c>
       <c r="D114" t="s">
+        <v>242</v>
+      </c>
+      <c r="E114" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+    <row r="115" spans="1:5">
+      <c r="A115">
         <v>116</v>
       </c>
       <c r="B115" t="s">
@@ -3161,11 +3579,14 @@
         <v>95</v>
       </c>
       <c r="D115" t="s">
+        <v>231</v>
+      </c>
+      <c r="E115" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
+    <row r="116" spans="1:5">
+      <c r="A116">
         <v>117</v>
       </c>
       <c r="B116" t="s">
@@ -3175,11 +3596,14 @@
         <v>57</v>
       </c>
       <c r="D116" t="s">
+        <v>243</v>
+      </c>
+      <c r="E116" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
+    <row r="117" spans="1:5">
+      <c r="A117">
         <v>118</v>
       </c>
       <c r="B117" t="s">
@@ -3189,11 +3613,14 @@
         <v>103</v>
       </c>
       <c r="D117" t="s">
+        <v>247</v>
+      </c>
+      <c r="E117" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
+    <row r="118" spans="1:5">
+      <c r="A118">
         <v>119</v>
       </c>
       <c r="B118" t="s">
@@ -3203,11 +3630,14 @@
         <v>46</v>
       </c>
       <c r="D118" t="s">
+        <v>237</v>
+      </c>
+      <c r="E118" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
+    <row r="119" spans="1:5">
+      <c r="A119">
         <v>120</v>
       </c>
       <c r="B119" t="s">
@@ -3217,11 +3647,14 @@
         <v>49</v>
       </c>
       <c r="D119" t="s">
+        <v>237</v>
+      </c>
+      <c r="E119" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
+    <row r="120" spans="1:5">
+      <c r="A120">
         <v>121</v>
       </c>
       <c r="B120" t="s">
@@ -3231,11 +3664,14 @@
         <v>45</v>
       </c>
       <c r="D120" t="s">
+        <v>237</v>
+      </c>
+      <c r="E120" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
+    <row r="121" spans="1:5">
+      <c r="A121">
         <v>122</v>
       </c>
       <c r="B121" t="s">
@@ -3245,11 +3681,14 @@
         <v>59</v>
       </c>
       <c r="D121" t="s">
+        <v>243</v>
+      </c>
+      <c r="E121" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
+    <row r="122" spans="1:5">
+      <c r="A122">
         <v>123</v>
       </c>
       <c r="B122" t="s">
@@ -3259,11 +3698,14 @@
         <v>62</v>
       </c>
       <c r="D122" t="s">
+        <v>243</v>
+      </c>
+      <c r="E122" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
+    <row r="123" spans="1:5">
+      <c r="A123">
         <v>124</v>
       </c>
       <c r="B123" t="s">
@@ -3273,11 +3715,14 @@
         <v>63</v>
       </c>
       <c r="D123" t="s">
+        <v>243</v>
+      </c>
+      <c r="E123" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
+    <row r="124" spans="1:5">
+      <c r="A124">
         <v>125</v>
       </c>
       <c r="B124" t="s">
@@ -3287,11 +3732,14 @@
         <v>5</v>
       </c>
       <c r="D124" t="s">
+        <v>236</v>
+      </c>
+      <c r="E124" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
+    <row r="125" spans="1:5">
+      <c r="A125">
         <v>126</v>
       </c>
       <c r="B125" t="s">
@@ -3301,11 +3749,14 @@
         <v>8</v>
       </c>
       <c r="D125" t="s">
+        <v>236</v>
+      </c>
+      <c r="E125" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
+    <row r="126" spans="1:5">
+      <c r="A126">
         <v>127</v>
       </c>
       <c r="B126" t="s">
@@ -3315,11 +3766,14 @@
         <v>115</v>
       </c>
       <c r="D126" t="s">
+        <v>239</v>
+      </c>
+      <c r="E126" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
+    <row r="127" spans="1:5">
+      <c r="A127">
         <v>128</v>
       </c>
       <c r="B127" t="s">
@@ -3329,17 +3783,25 @@
         <v>61</v>
       </c>
       <c r="D127" t="s">
+        <v>243</v>
+      </c>
+      <c r="E127" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1">
+  <autoFilter ref="A1:E1">
     <sortState ref="A2:D127">
       <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3349,8 +3811,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>